<commit_message>
Diagramas y Plantilla tareas
Se registraron los tiempos de las tareas completadas, además se agrego los diagramas de robustez y de secuencia
</commit_message>
<xml_diff>
--- a/Documentos/Tareas/Iteración_2 Registro.xlsx
+++ b/Documentos/Tareas/Iteración_2 Registro.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Documents\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-REX\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AB4788-79B0-4105-9114-52B16DFBAD62}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -951,10 +952,10 @@
   <dimension ref="B1:BA54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="L24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1976,7 +1977,7 @@
         <v>52</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="G12" s="30">
         <v>2</v>
@@ -1993,90 +1994,92 @@
         <v>2</v>
       </c>
       <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
+      <c r="N12" s="31">
+        <v>2</v>
+      </c>
       <c r="O12" s="31">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P12" s="31"/>
       <c r="Q12" s="31"/>
       <c r="R12" s="31">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S12" s="31"/>
       <c r="T12" s="31"/>
       <c r="U12" s="31">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V12" s="31"/>
       <c r="W12" s="31"/>
       <c r="X12" s="31">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="31"/>
       <c r="Z12" s="31"/>
       <c r="AA12" s="31">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB12" s="31"/>
       <c r="AC12" s="31"/>
       <c r="AD12" s="31">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE12" s="31"/>
       <c r="AF12" s="31"/>
       <c r="AG12" s="31">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH12" s="31"/>
       <c r="AI12" s="31"/>
       <c r="AJ12" s="31">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK12" s="31"/>
       <c r="AL12" s="31"/>
       <c r="AM12" s="31">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN12" s="31"/>
       <c r="AO12" s="31"/>
       <c r="AP12" s="31">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ12" s="31"/>
       <c r="AR12" s="31"/>
       <c r="AS12" s="31">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT12" s="31"/>
       <c r="AU12" s="31"/>
       <c r="AV12" s="31">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW12" s="31"/>
       <c r="AX12" s="31"/>
       <c r="AY12" s="31">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ12" s="31">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA12" s="31">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:53" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -2707,46 +2710,48 @@
         <v>1</v>
       </c>
       <c r="S18" s="31"/>
-      <c r="T18" s="31"/>
+      <c r="T18" s="31">
+        <v>2</v>
+      </c>
       <c r="U18" s="31">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V18" s="31"/>
       <c r="W18" s="31"/>
       <c r="X18" s="31">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y18" s="31"/>
       <c r="Z18" s="31"/>
       <c r="AA18" s="31">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB18" s="31"/>
       <c r="AC18" s="31"/>
       <c r="AD18" s="31">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AE18" s="31"/>
       <c r="AF18" s="31"/>
       <c r="AG18" s="31">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AH18" s="31"/>
       <c r="AI18" s="31"/>
       <c r="AJ18" s="31">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AK18" s="31"/>
       <c r="AL18" s="31"/>
       <c r="AM18" s="31">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AN18" s="31"/>
       <c r="AO18" s="31">
@@ -2754,13 +2759,13 @@
       </c>
       <c r="AP18" s="31">
         <f t="shared" si="10"/>
-        <v>0.75</v>
+        <v>-1.25</v>
       </c>
       <c r="AQ18" s="31"/>
       <c r="AR18" s="31"/>
       <c r="AS18" s="31">
         <f t="shared" si="11"/>
-        <v>0.75</v>
+        <v>-1.25</v>
       </c>
       <c r="AT18" s="31"/>
       <c r="AU18" s="31">
@@ -2768,21 +2773,21 @@
       </c>
       <c r="AV18" s="31">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="AW18" s="31"/>
       <c r="AX18" s="31"/>
       <c r="AY18" s="31">
         <f t="shared" si="13"/>
-        <v>0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="AZ18" s="31">
         <f t="shared" si="14"/>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="BA18" s="31">
         <f t="shared" si="15"/>
-        <v>0.5</v>
+        <v>-1.5</v>
       </c>
     </row>
     <row r="19" spans="2:53" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -2828,58 +2833,60 @@
         <v>1</v>
       </c>
       <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
+      <c r="T19" s="31">
+        <v>1</v>
+      </c>
       <c r="U19" s="31">
         <f t="shared" ref="U19" si="116">R19-T19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V19" s="31"/>
       <c r="W19" s="31"/>
       <c r="X19" s="31">
         <f t="shared" ref="X19" si="117">U19-W19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y19" s="31"/>
       <c r="Z19" s="31"/>
       <c r="AA19" s="31">
         <f t="shared" ref="AA19" si="118">X19-Z19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB19" s="31"/>
       <c r="AC19" s="31"/>
       <c r="AD19" s="31">
         <f t="shared" ref="AD19" si="119">AA19-AC19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE19" s="31"/>
       <c r="AF19" s="31"/>
       <c r="AG19" s="31">
         <f t="shared" ref="AG19" si="120">AD19-AF19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH19" s="31"/>
       <c r="AI19" s="31"/>
       <c r="AJ19" s="31">
         <f t="shared" ref="AJ19" si="121">AG19-AI19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK19" s="31"/>
       <c r="AL19" s="31"/>
       <c r="AM19" s="31">
         <f t="shared" ref="AM19" si="122">AJ19-AL19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN19" s="31"/>
       <c r="AO19" s="31"/>
       <c r="AP19" s="31">
         <f t="shared" ref="AP19" si="123">AM19-AO19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ19" s="31"/>
       <c r="AR19" s="31"/>
       <c r="AS19" s="31">
         <f t="shared" ref="AS19" si="124">AP19-AR19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT19" s="31"/>
       <c r="AU19" s="31">
@@ -2887,7 +2894,7 @@
       </c>
       <c r="AV19" s="31">
         <f t="shared" ref="AV19" si="125">AS19-AU19</f>
-        <v>0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="AW19" s="31"/>
       <c r="AX19" s="31">
@@ -2895,15 +2902,15 @@
       </c>
       <c r="AY19" s="31">
         <f t="shared" ref="AY19" si="126">AV19-AX19</f>
-        <v>0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="AZ19" s="31">
         <f t="shared" ref="AZ19" si="127">H19+K19+N19+Q19+T19+W19+Z19+AC19+AF19+AI19+AL19+AO19+AR19+AU19+AX19</f>
-        <v>0.75</v>
+        <v>1.75</v>
       </c>
       <c r="BA19" s="31">
         <f t="shared" ref="BA19" si="128">G19-AZ19</f>
-        <v>0.25</v>
+        <v>-0.75</v>
       </c>
     </row>
     <row r="20" spans="2:53" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -2949,78 +2956,80 @@
         <v>1</v>
       </c>
       <c r="S20" s="31"/>
-      <c r="T20" s="31"/>
+      <c r="T20" s="31">
+        <v>1</v>
+      </c>
       <c r="U20" s="31">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V20" s="31"/>
       <c r="W20" s="31"/>
       <c r="X20" s="31">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y20" s="31"/>
       <c r="Z20" s="31"/>
       <c r="AA20" s="31">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB20" s="31"/>
       <c r="AC20" s="31"/>
       <c r="AD20" s="31">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE20" s="31"/>
       <c r="AF20" s="31"/>
       <c r="AG20" s="31">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH20" s="31"/>
       <c r="AI20" s="31"/>
       <c r="AJ20" s="31">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK20" s="31"/>
       <c r="AL20" s="31"/>
       <c r="AM20" s="31">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN20" s="31"/>
       <c r="AO20" s="31"/>
       <c r="AP20" s="31">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ20" s="31"/>
       <c r="AR20" s="31"/>
       <c r="AS20" s="31">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT20" s="31"/>
       <c r="AU20" s="31"/>
       <c r="AV20" s="31">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW20" s="31"/>
       <c r="AX20" s="31"/>
       <c r="AY20" s="31">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ20" s="31">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA20" s="31">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:53" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -3747,7 +3756,7 @@
         <v>52</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G27" s="30">
         <v>1</v>
@@ -3776,78 +3785,80 @@
         <v>1</v>
       </c>
       <c r="S27" s="31"/>
-      <c r="T27" s="31"/>
+      <c r="T27" s="31">
+        <v>2</v>
+      </c>
       <c r="U27" s="31">
         <f t="shared" ref="U27:U29" si="180">R27-T27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V27" s="31"/>
       <c r="W27" s="31"/>
       <c r="X27" s="31">
         <f t="shared" ref="X27:X29" si="181">U27-W27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y27" s="31"/>
       <c r="Z27" s="31"/>
       <c r="AA27" s="31">
         <f t="shared" ref="AA27:AA29" si="182">X27-Z27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB27" s="31"/>
       <c r="AC27" s="31"/>
       <c r="AD27" s="31">
         <f t="shared" ref="AD27:AD29" si="183">AA27-AC27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AE27" s="31"/>
       <c r="AF27" s="31"/>
       <c r="AG27" s="31">
         <f t="shared" ref="AG27:AG29" si="184">AD27-AF27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AH27" s="31"/>
       <c r="AI27" s="31"/>
       <c r="AJ27" s="31">
         <f t="shared" ref="AJ27:AJ29" si="185">AG27-AI27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AK27" s="31"/>
       <c r="AL27" s="31"/>
       <c r="AM27" s="31">
         <f t="shared" ref="AM27:AM29" si="186">AJ27-AL27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AN27" s="31"/>
       <c r="AO27" s="31"/>
       <c r="AP27" s="31">
         <f t="shared" ref="AP27:AP29" si="187">AM27-AO27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AQ27" s="31"/>
       <c r="AR27" s="31"/>
       <c r="AS27" s="31">
         <f t="shared" ref="AS27:AS29" si="188">AP27-AR27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AT27" s="31"/>
       <c r="AU27" s="31"/>
       <c r="AV27" s="31">
         <f t="shared" ref="AV27:AV29" si="189">AS27-AU27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AW27" s="31"/>
       <c r="AX27" s="31"/>
       <c r="AY27" s="31">
         <f t="shared" ref="AY27:AY29" si="190">AV27-AX27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AZ27" s="31">
         <f t="shared" ref="AZ27:AZ29" si="191">H27+K27+N27+Q27+T27+W27+Z27+AC27+AF27+AI27+AL27+AO27+AR27+AU27+AX27</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA27" s="31">
         <f t="shared" ref="BA27:BA29" si="192">G27-AZ27</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="28" spans="2:53" s="32" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Diagramas de secuencia y Pantilla
Se agregaron los diagramas de secuencia de los casos de uso administrar grupo, administrar profesor, consultar ingresos. Además se actualizó la plantilla de tareas
</commit_message>
<xml_diff>
--- a/Documentos/Tareas/Iteración_2 Registro.xlsx
+++ b/Documentos/Tareas/Iteración_2 Registro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-REX\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AB4788-79B0-4105-9114-52B16DFBAD62}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD422D42-A09A-451C-BC07-A27E1183AF73}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -952,10 +952,10 @@
   <dimension ref="B1:BA54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,40 +2754,36 @@
         <v>-1</v>
       </c>
       <c r="AN18" s="31"/>
-      <c r="AO18" s="31">
-        <v>0.25</v>
-      </c>
+      <c r="AO18" s="31"/>
       <c r="AP18" s="31">
         <f t="shared" si="10"/>
-        <v>-1.25</v>
+        <v>-1</v>
       </c>
       <c r="AQ18" s="31"/>
       <c r="AR18" s="31"/>
       <c r="AS18" s="31">
         <f t="shared" si="11"/>
-        <v>-1.25</v>
+        <v>-1</v>
       </c>
       <c r="AT18" s="31"/>
-      <c r="AU18" s="31">
-        <v>0.25</v>
-      </c>
+      <c r="AU18" s="31"/>
       <c r="AV18" s="31">
         <f t="shared" si="12"/>
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="AW18" s="31"/>
       <c r="AX18" s="31"/>
       <c r="AY18" s="31">
         <f t="shared" si="13"/>
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="AZ18" s="31">
         <f t="shared" si="14"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="BA18" s="31">
         <f t="shared" si="15"/>
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="19" spans="2:53" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -2889,28 +2885,24 @@
         <v>0</v>
       </c>
       <c r="AT19" s="31"/>
-      <c r="AU19" s="31">
-        <v>0.25</v>
-      </c>
+      <c r="AU19" s="31"/>
       <c r="AV19" s="31">
         <f t="shared" ref="AV19" si="125">AS19-AU19</f>
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="AW19" s="31"/>
-      <c r="AX19" s="31">
-        <v>0.5</v>
-      </c>
+      <c r="AX19" s="31"/>
       <c r="AY19" s="31">
         <f t="shared" ref="AY19" si="126">AV19-AX19</f>
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="AZ19" s="31">
         <f t="shared" ref="AZ19" si="127">H19+K19+N19+Q19+T19+W19+Z19+AC19+AF19+AI19+AL19+AO19+AR19+AU19+AX19</f>
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="BA19" s="31">
         <f t="shared" ref="BA19" si="128">G19-AZ19</f>
-        <v>-0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:53" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3875,7 +3867,7 @@
         <v>52</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G28" s="30">
         <v>1</v>
@@ -3940,46 +3932,44 @@
         <v>1</v>
       </c>
       <c r="AK28" s="31"/>
-      <c r="AL28" s="31"/>
+      <c r="AL28" s="31">
+        <v>0.8</v>
+      </c>
       <c r="AM28" s="31">
         <f t="shared" si="186"/>
-        <v>1</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AN28" s="31"/>
-      <c r="AO28" s="31">
-        <v>0.25</v>
-      </c>
+      <c r="AO28" s="31"/>
       <c r="AP28" s="31">
         <f t="shared" si="187"/>
-        <v>0.75</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AQ28" s="31"/>
       <c r="AR28" s="31"/>
       <c r="AS28" s="31">
         <f t="shared" si="188"/>
-        <v>0.75</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AT28" s="31"/>
-      <c r="AU28" s="31">
-        <v>0.15</v>
-      </c>
+      <c r="AU28" s="31"/>
       <c r="AV28" s="31">
         <f t="shared" si="189"/>
-        <v>0.6</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AW28" s="31"/>
       <c r="AX28" s="31"/>
       <c r="AY28" s="31">
         <f t="shared" si="190"/>
-        <v>0.6</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AZ28" s="31">
         <f t="shared" si="191"/>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="BA28" s="31">
         <f t="shared" si="192"/>
-        <v>0.6</v>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="29" spans="2:53" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3996,7 +3986,7 @@
         <v>52</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G29" s="30">
         <v>1</v>
@@ -4061,46 +4051,44 @@
         <v>1</v>
       </c>
       <c r="AK29" s="31"/>
-      <c r="AL29" s="31"/>
+      <c r="AL29" s="31">
+        <v>0.8</v>
+      </c>
       <c r="AM29" s="31">
         <f t="shared" si="186"/>
-        <v>1</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AN29" s="31"/>
       <c r="AO29" s="31"/>
       <c r="AP29" s="31">
         <f t="shared" si="187"/>
-        <v>1</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AQ29" s="31"/>
       <c r="AR29" s="31"/>
       <c r="AS29" s="31">
         <f t="shared" si="188"/>
-        <v>1</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AT29" s="31"/>
-      <c r="AU29" s="31">
-        <v>0.25</v>
-      </c>
+      <c r="AU29" s="31"/>
       <c r="AV29" s="31">
         <f t="shared" si="189"/>
-        <v>0.75</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AW29" s="31"/>
-      <c r="AX29" s="31">
-        <v>0.15</v>
-      </c>
+      <c r="AX29" s="31"/>
       <c r="AY29" s="31">
         <f t="shared" si="190"/>
-        <v>0.6</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AZ29" s="31">
         <f t="shared" si="191"/>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="BA29" s="31">
         <f t="shared" si="192"/>
-        <v>0.6</v>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="30" spans="2:53" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -4357,7 +4345,7 @@
         <v>52</v>
       </c>
       <c r="F32" s="29" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G32" s="30">
         <v>1</v>
@@ -4410,21 +4398,21 @@
         <v>1</v>
       </c>
       <c r="AE32" s="31"/>
-      <c r="AF32" s="31">
-        <v>0.8</v>
-      </c>
+      <c r="AF32" s="31"/>
       <c r="AG32" s="31">
         <f t="shared" ref="AG32:AG41" si="217">AD32-AF32</f>
-        <v>0.19999999999999996</v>
+        <v>1</v>
       </c>
       <c r="AH32" s="31"/>
       <c r="AI32" s="31"/>
       <c r="AJ32" s="31">
         <f t="shared" ref="AJ32:AJ41" si="218">AG32-AI32</f>
-        <v>0.19999999999999996</v>
+        <v>1</v>
       </c>
       <c r="AK32" s="31"/>
-      <c r="AL32" s="31"/>
+      <c r="AL32" s="31">
+        <v>0.8</v>
+      </c>
       <c r="AM32" s="31">
         <f t="shared" ref="AM32:AM41" si="219">AJ32-AL32</f>
         <v>0.19999999999999996</v>
@@ -4442,26 +4430,24 @@
         <v>0.19999999999999996</v>
       </c>
       <c r="AT32" s="31"/>
-      <c r="AU32" s="31">
-        <v>0.15</v>
-      </c>
+      <c r="AU32" s="31"/>
       <c r="AV32" s="31">
         <f t="shared" ref="AV32:AV41" si="222">AS32-AU32</f>
-        <v>4.9999999999999961E-2</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AW32" s="31"/>
       <c r="AX32" s="31"/>
       <c r="AY32" s="31">
         <f t="shared" ref="AY32:AY41" si="223">AV32-AX32</f>
-        <v>4.9999999999999961E-2</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="AZ32" s="31">
         <f>H32+K32+N32+Q32+T32+W32+Z32+AC32+AF32+AI32+AL32+AO32+AR32+AU32+AX32</f>
-        <v>0.95000000000000007</v>
+        <v>0.8</v>
       </c>
       <c r="BA32" s="31">
         <f t="shared" ref="BA32:BA41" si="224">G32-AZ32</f>
-        <v>4.9999999999999933E-2</v>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="33" spans="2:53" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -6893,11 +6879,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -6909,6 +6890,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Descripción de CU - 24  Diagramas de secuencia y robustez
</commit_message>
<xml_diff>
--- a/Documentos/Tareas/Iteración_2 Registro.xlsx
+++ b/Documentos/Tareas/Iteración_2 Registro.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-REX\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Documents\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD422D42-A09A-451C-BC07-A27E1183AF73}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="97">
   <si>
     <t>Columna</t>
   </si>
@@ -952,10 +951,10 @@
   <dimension ref="B1:BA54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AI30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3690,48 +3689,50 @@
         <v>1</v>
       </c>
       <c r="AH26" s="34"/>
-      <c r="AI26" s="34"/>
+      <c r="AI26" s="34">
+        <v>0.5</v>
+      </c>
       <c r="AJ26" s="34">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AK26" s="34"/>
       <c r="AL26" s="34"/>
       <c r="AM26" s="34">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN26" s="34"/>
       <c r="AO26" s="34"/>
       <c r="AP26" s="34">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ26" s="34"/>
       <c r="AR26" s="34"/>
       <c r="AS26" s="34">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AT26" s="34"/>
       <c r="AU26" s="34"/>
       <c r="AV26" s="34">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW26" s="34"/>
       <c r="AX26" s="34"/>
       <c r="AY26" s="34">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ26" s="34">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA26" s="34">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="2:53" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -4273,62 +4274,64 @@
         <v>1</v>
       </c>
       <c r="AB31" s="34"/>
-      <c r="AC31" s="34"/>
+      <c r="AC31" s="34">
+        <v>0.5</v>
+      </c>
       <c r="AD31" s="34">
         <f t="shared" si="199"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AE31" s="34"/>
       <c r="AF31" s="34"/>
       <c r="AG31" s="34">
         <f t="shared" si="200"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AH31" s="34"/>
       <c r="AI31" s="34"/>
       <c r="AJ31" s="34">
         <f t="shared" si="201"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AK31" s="34"/>
-      <c r="AL31" s="34"/>
+      <c r="AL31" s="34">
+        <v>1</v>
+      </c>
       <c r="AM31" s="34">
         <f t="shared" si="202"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AN31" s="34"/>
       <c r="AO31" s="34"/>
       <c r="AP31" s="34">
         <f t="shared" si="203"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AQ31" s="34"/>
-      <c r="AR31" s="34">
-        <v>0.25</v>
-      </c>
+      <c r="AR31" s="34"/>
       <c r="AS31" s="34">
         <f t="shared" si="204"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AT31" s="34"/>
       <c r="AU31" s="34"/>
       <c r="AV31" s="34">
         <f t="shared" si="205"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AW31" s="34"/>
       <c r="AX31" s="34"/>
       <c r="AY31" s="34">
         <f t="shared" si="206"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AZ31" s="34">
         <f t="shared" si="207"/>
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="BA31" s="34">
         <f t="shared" si="208"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="32" spans="2:53" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -4464,7 +4467,7 @@
         <v>54</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G33" s="24">
         <v>1</v>
@@ -4585,7 +4588,7 @@
         <v>53</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G34" s="33">
         <v>1</v>
@@ -4658,16 +4661,18 @@
         <v>0.5</v>
       </c>
       <c r="AN34" s="34"/>
-      <c r="AO34" s="34"/>
+      <c r="AO34" s="34">
+        <v>0.5</v>
+      </c>
       <c r="AP34" s="34">
         <f t="shared" si="220"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AQ34" s="34"/>
       <c r="AR34" s="34"/>
       <c r="AS34" s="34">
         <f t="shared" si="221"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AT34" s="34"/>
       <c r="AU34" s="34">
@@ -4675,21 +4680,21 @@
       </c>
       <c r="AV34" s="34">
         <f t="shared" si="222"/>
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="AW34" s="34"/>
       <c r="AX34" s="34"/>
       <c r="AY34" s="34">
         <f t="shared" si="223"/>
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="AZ34" s="34">
         <f>H34+K34+N34+Q34+T34+W34+Z34+AC34+AF34+AI34+AL34+AO34+AR34+AU34+AX34</f>
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="BA34" s="34">
         <f t="shared" si="224"/>
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="35" spans="2:53" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -4706,7 +4711,7 @@
         <v>53</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G35" s="33">
         <v>1</v>
@@ -4777,16 +4782,18 @@
         <v>1</v>
       </c>
       <c r="AN35" s="34"/>
-      <c r="AO35" s="34"/>
+      <c r="AO35" s="34">
+        <v>1</v>
+      </c>
       <c r="AP35" s="34">
         <f t="shared" si="220"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ35" s="34"/>
       <c r="AR35" s="34"/>
       <c r="AS35" s="34">
         <f t="shared" si="221"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT35" s="34"/>
       <c r="AU35" s="34">
@@ -4794,21 +4801,21 @@
       </c>
       <c r="AV35" s="34">
         <f t="shared" si="222"/>
-        <v>0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="AW35" s="34"/>
       <c r="AX35" s="34"/>
       <c r="AY35" s="34">
         <f t="shared" si="223"/>
-        <v>0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="AZ35" s="34">
         <f t="shared" ref="AZ35" si="226">H35+K35+N35+Q35+T35+W35+Z35+AC35+AF35+AI35+AL35+AO35+AR35+AU35+AX35</f>
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="BA35" s="34">
         <f t="shared" si="224"/>
-        <v>0.75</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="36" spans="2:53" x14ac:dyDescent="0.25">
@@ -5533,7 +5540,7 @@
         <v>53</v>
       </c>
       <c r="F42" s="39" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G42" s="40">
         <v>1</v>
@@ -5594,28 +5601,30 @@
         <v>0.75</v>
       </c>
       <c r="AH42" s="41"/>
-      <c r="AI42" s="41"/>
+      <c r="AI42" s="41">
+        <v>0.5</v>
+      </c>
       <c r="AJ42" s="41">
         <f t="shared" ref="AJ42:AJ46" si="239">AG42-AI42</f>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="AK42" s="41"/>
       <c r="AL42" s="41"/>
       <c r="AM42" s="41">
         <f t="shared" ref="AM42:AM46" si="240">AJ42-AL42</f>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="AN42" s="41"/>
       <c r="AO42" s="41"/>
       <c r="AP42" s="41">
         <f t="shared" ref="AP42:AP46" si="241">AM42-AO42</f>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="AQ42" s="41"/>
       <c r="AR42" s="41"/>
       <c r="AS42" s="41">
         <f t="shared" ref="AS42:AS46" si="242">AP42-AR42</f>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="AT42" s="41"/>
       <c r="AU42" s="41">
@@ -5623,21 +5632,21 @@
       </c>
       <c r="AV42" s="41">
         <f t="shared" ref="AV42:AV46" si="243">AS42-AU42</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AW42" s="41"/>
       <c r="AX42" s="41"/>
       <c r="AY42" s="41">
         <f t="shared" ref="AY42:AY46" si="244">AV42-AX42</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AZ42" s="41">
         <f>H42+K42+N42+Q42+T42+W42+Z42+AC42+AF42+AI42+AL42+AO42+AR42+AU42+AX42</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="BA42" s="41">
         <f t="shared" ref="BA42:BA46" si="245">G42-AZ42</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:53" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -5654,7 +5663,7 @@
         <v>53</v>
       </c>
       <c r="F43" s="39" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G43" s="43">
         <v>1</v>
@@ -5713,157 +5722,171 @@
         <v>1</v>
       </c>
       <c r="AH43" s="41"/>
-      <c r="AI43" s="41"/>
+      <c r="AI43" s="41">
+        <v>0.7</v>
+      </c>
       <c r="AJ43" s="41">
         <f t="shared" si="239"/>
-        <v>1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AK43" s="41"/>
       <c r="AL43" s="41"/>
       <c r="AM43" s="41">
         <f t="shared" si="240"/>
-        <v>1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AN43" s="41"/>
       <c r="AO43" s="41"/>
       <c r="AP43" s="41">
         <f t="shared" si="241"/>
-        <v>1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AQ43" s="41"/>
       <c r="AR43" s="41"/>
       <c r="AS43" s="41">
         <f t="shared" si="242"/>
-        <v>1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AT43" s="41"/>
       <c r="AU43" s="41"/>
       <c r="AV43" s="41">
         <f t="shared" si="243"/>
-        <v>1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AW43" s="41"/>
       <c r="AX43" s="41"/>
       <c r="AY43" s="41">
         <f t="shared" si="244"/>
-        <v>1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AZ43" s="41">
         <f t="shared" ref="AZ43" si="246">H43+K43+N43+Q43+T43+W43+Z43+AC43+AF43+AI43+AL43+AO43+AR43+AU43+AX43</f>
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="BA43" s="41">
         <f t="shared" si="245"/>
-        <v>1</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="44" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B44" s="13"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8">
+    <row r="44" spans="2:53" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="F44" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="G44" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41">
         <f t="shared" si="230"/>
-        <v>0</v>
-      </c>
-      <c r="J44" s="10"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="J44" s="41"/>
+      <c r="K44" s="41"/>
+      <c r="L44" s="41">
         <f t="shared" si="231"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="10"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M44" s="41"/>
+      <c r="N44" s="41"/>
+      <c r="O44" s="41">
         <f t="shared" si="232"/>
-        <v>0</v>
-      </c>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="P44" s="41"/>
+      <c r="Q44" s="41"/>
+      <c r="R44" s="41">
         <f t="shared" si="233"/>
-        <v>0</v>
-      </c>
-      <c r="S44" s="10"/>
-      <c r="T44" s="8"/>
-      <c r="U44" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="S44" s="41"/>
+      <c r="T44" s="41"/>
+      <c r="U44" s="41">
         <f t="shared" si="234"/>
-        <v>0</v>
-      </c>
-      <c r="V44" s="10"/>
-      <c r="W44" s="8"/>
-      <c r="X44" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="V44" s="41"/>
+      <c r="W44" s="41"/>
+      <c r="X44" s="41">
         <f t="shared" si="235"/>
-        <v>0</v>
-      </c>
-      <c r="Y44" s="10"/>
-      <c r="Z44" s="8"/>
-      <c r="AA44" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="Y44" s="41"/>
+      <c r="Z44" s="41"/>
+      <c r="AA44" s="41">
         <f t="shared" si="236"/>
-        <v>0</v>
-      </c>
-      <c r="AB44" s="10"/>
-      <c r="AC44" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="AB44" s="41"/>
+      <c r="AC44" s="41">
         <v>0.25</v>
       </c>
-      <c r="AD44" s="8">
+      <c r="AD44" s="41">
         <f t="shared" si="237"/>
-        <v>-0.25</v>
-      </c>
-      <c r="AE44" s="10"/>
-      <c r="AF44" s="8"/>
-      <c r="AG44" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="AE44" s="41"/>
+      <c r="AF44" s="41"/>
+      <c r="AG44" s="41">
         <f t="shared" si="238"/>
-        <v>-0.25</v>
-      </c>
-      <c r="AH44" s="10"/>
-      <c r="AI44" s="8"/>
-      <c r="AJ44" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="AH44" s="41"/>
+      <c r="AI44" s="41"/>
+      <c r="AJ44" s="41">
         <f t="shared" si="239"/>
-        <v>-0.25</v>
-      </c>
-      <c r="AK44" s="10"/>
-      <c r="AL44" s="8"/>
-      <c r="AM44" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="AK44" s="41"/>
+      <c r="AL44" s="41"/>
+      <c r="AM44" s="41">
         <f t="shared" si="240"/>
-        <v>-0.25</v>
-      </c>
-      <c r="AN44" s="10"/>
-      <c r="AO44" s="8"/>
-      <c r="AP44" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="AN44" s="41"/>
+      <c r="AO44" s="41"/>
+      <c r="AP44" s="41">
         <f t="shared" si="241"/>
-        <v>-0.25</v>
-      </c>
-      <c r="AQ44" s="10"/>
-      <c r="AR44" s="8"/>
-      <c r="AS44" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="AQ44" s="41"/>
+      <c r="AR44" s="41"/>
+      <c r="AS44" s="41">
         <f t="shared" si="242"/>
-        <v>-0.25</v>
-      </c>
-      <c r="AT44" s="10"/>
-      <c r="AU44" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="AT44" s="41"/>
+      <c r="AU44" s="41">
         <v>0.15</v>
       </c>
-      <c r="AV44" s="8">
+      <c r="AV44" s="41">
         <f t="shared" si="243"/>
-        <v>-0.4</v>
-      </c>
-      <c r="AW44" s="10"/>
-      <c r="AX44" s="8"/>
-      <c r="AY44" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="AW44" s="41"/>
+      <c r="AX44" s="41"/>
+      <c r="AY44" s="41">
         <f t="shared" si="244"/>
-        <v>-0.4</v>
-      </c>
-      <c r="AZ44" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="AZ44" s="41">
         <f>H44+K44+N44+Q44+T44+W44+Z44+AC44+AF44+AI44+AL44+AO44+AR44+AU44+AX44</f>
         <v>0.4</v>
       </c>
-      <c r="BA44" s="11">
+      <c r="BA44" s="41">
         <f t="shared" si="245"/>
-        <v>-0.4</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="45" spans="2:53" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Interfaces de los CU Inscribir alumno y Dar de baja alumno, generacion de imagenes de diagramas.
Se realizaron las interfaces graficas de los CU Inscribir alumno y Dar de baja alumno, se generaron las imagenes de los diagramas de robustez y secuencia.
</commit_message>
<xml_diff>
--- a/Documentos/Tareas/Iteración_2 Registro.xlsx
+++ b/Documentos/Tareas/Iteración_2 Registro.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Documents\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymu\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BDF962-6908-4247-BCEC-9A0018B53793}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -951,10 +952,10 @@
   <dimension ref="B1:BA54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AI30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AI6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomRight" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,7 +1858,7 @@
         <v>54</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="G11" s="24">
         <v>2</v>
@@ -1874,94 +1875,92 @@
         <v>2</v>
       </c>
       <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
+      <c r="N11" s="25">
+        <v>1.5</v>
+      </c>
       <c r="O11" s="25">
         <f t="shared" ref="O11" si="50">L11-N11</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P11" s="25"/>
       <c r="Q11" s="25"/>
       <c r="R11" s="25">
         <f t="shared" ref="R11" si="51">O11-Q11</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="S11" s="25"/>
       <c r="T11" s="25"/>
       <c r="U11" s="25">
         <f t="shared" ref="U11" si="52">R11-T11</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="V11" s="25"/>
       <c r="W11" s="25"/>
       <c r="X11" s="25">
         <f t="shared" ref="X11" si="53">U11-W11</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="Y11" s="25"/>
       <c r="Z11" s="25"/>
       <c r="AA11" s="25">
         <f t="shared" ref="AA11" si="54">X11-Z11</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AB11" s="25"/>
       <c r="AC11" s="25"/>
       <c r="AD11" s="25">
         <f t="shared" ref="AD11" si="55">AA11-AC11</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AE11" s="25"/>
       <c r="AF11" s="25"/>
       <c r="AG11" s="25">
         <f t="shared" ref="AG11" si="56">AD11-AF11</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AH11" s="25"/>
       <c r="AI11" s="25"/>
       <c r="AJ11" s="25">
         <f t="shared" ref="AJ11" si="57">AG11-AI11</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AK11" s="25"/>
       <c r="AL11" s="25"/>
       <c r="AM11" s="25">
         <f t="shared" ref="AM11" si="58">AJ11-AL11</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AN11" s="25"/>
       <c r="AO11" s="25"/>
       <c r="AP11" s="25">
         <f t="shared" ref="AP11" si="59">AM11-AO11</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AQ11" s="25"/>
       <c r="AR11" s="25"/>
       <c r="AS11" s="25">
         <f t="shared" ref="AS11" si="60">AP11-AR11</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AT11" s="25"/>
-      <c r="AU11" s="25">
-        <v>0.5</v>
-      </c>
+      <c r="AU11" s="25"/>
       <c r="AV11" s="25">
         <f t="shared" ref="AV11" si="61">AS11-AU11</f>
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="AW11" s="25"/>
-      <c r="AX11" s="25">
-        <v>0.25</v>
-      </c>
+      <c r="AX11" s="25"/>
       <c r="AY11" s="25">
         <f t="shared" ref="AY11" si="62">AV11-AX11</f>
-        <v>1.25</v>
+        <v>0.5</v>
       </c>
       <c r="AZ11" s="25">
         <f t="shared" ref="AZ11" si="63">H11+K11+N11+Q11+T11+W11+Z11+AC11+AF11+AI11+AL11+AO11+AR11+AU11+AX11</f>
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="BA11" s="25">
         <f t="shared" ref="BA11" si="64">G11-AZ11</f>
-        <v>1.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="2:53" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3037,7 +3036,7 @@
         <v>54</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G21" s="24">
         <v>1</v>
@@ -3072,72 +3071,74 @@
         <v>1</v>
       </c>
       <c r="V21" s="25"/>
-      <c r="W21" s="25"/>
+      <c r="W21" s="25">
+        <v>0.5</v>
+      </c>
       <c r="X21" s="25">
         <f t="shared" ref="X21" si="133">U21-W21</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y21" s="25"/>
       <c r="Z21" s="25"/>
       <c r="AA21" s="25">
         <f t="shared" ref="AA21" si="134">X21-Z21</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AB21" s="25"/>
       <c r="AC21" s="25"/>
       <c r="AD21" s="25">
         <f t="shared" ref="AD21" si="135">AA21-AC21</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AE21" s="25"/>
       <c r="AF21" s="25"/>
       <c r="AG21" s="25">
         <f t="shared" ref="AG21" si="136">AD21-AF21</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AH21" s="25"/>
       <c r="AI21" s="25"/>
       <c r="AJ21" s="25">
         <f t="shared" ref="AJ21" si="137">AG21-AI21</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AK21" s="25"/>
       <c r="AL21" s="25"/>
       <c r="AM21" s="25">
         <f t="shared" ref="AM21" si="138">AJ21-AL21</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN21" s="25"/>
       <c r="AO21" s="25"/>
       <c r="AP21" s="25">
         <f t="shared" ref="AP21" si="139">AM21-AO21</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ21" s="25"/>
       <c r="AR21" s="25"/>
       <c r="AS21" s="25">
         <f t="shared" ref="AS21" si="140">AP21-AR21</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AT21" s="25"/>
       <c r="AU21" s="25"/>
       <c r="AV21" s="25">
         <f t="shared" ref="AV21" si="141">AS21-AU21</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW21" s="25"/>
       <c r="AX21" s="25"/>
       <c r="AY21" s="25">
         <f t="shared" ref="AY21" si="142">AV21-AX21</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ21" s="25">
         <f t="shared" ref="AZ21" si="143">H21+K21+N21+Q21+T21+W21+Z21+AC21+AF21+AI21+AL21+AO21+AR21+AU21+AX21</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA21" s="25">
         <f t="shared" ref="BA21" si="144">G21-AZ21</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="2:53" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -3413,86 +3414,88 @@
         <v>1</v>
       </c>
       <c r="P24" s="25"/>
-      <c r="Q24" s="25"/>
+      <c r="Q24" s="25">
+        <v>2</v>
+      </c>
       <c r="R24" s="25">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S24" s="25"/>
       <c r="T24" s="25"/>
       <c r="U24" s="25">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V24" s="25"/>
-      <c r="W24" s="25"/>
+      <c r="W24" s="25">
+        <v>0.5</v>
+      </c>
       <c r="X24" s="25">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-1.5</v>
       </c>
       <c r="Y24" s="25"/>
       <c r="Z24" s="25"/>
       <c r="AA24" s="25">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>-1.5</v>
       </c>
       <c r="AB24" s="25"/>
       <c r="AC24" s="25"/>
       <c r="AD24" s="25">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>-1.5</v>
       </c>
       <c r="AE24" s="25"/>
       <c r="AF24" s="25"/>
       <c r="AG24" s="25">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-1.5</v>
       </c>
       <c r="AH24" s="25"/>
       <c r="AI24" s="25"/>
       <c r="AJ24" s="25">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1.5</v>
       </c>
       <c r="AK24" s="25"/>
       <c r="AL24" s="25"/>
       <c r="AM24" s="25">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1.5</v>
       </c>
       <c r="AN24" s="25"/>
       <c r="AO24" s="25"/>
       <c r="AP24" s="25">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>-1.5</v>
       </c>
       <c r="AQ24" s="25"/>
       <c r="AR24" s="25"/>
       <c r="AS24" s="25">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>-1.5</v>
       </c>
       <c r="AT24" s="25"/>
-      <c r="AU24" s="25">
-        <v>0.15</v>
-      </c>
+      <c r="AU24" s="25"/>
       <c r="AV24" s="25">
         <f t="shared" si="12"/>
-        <v>0.85</v>
+        <v>-1.5</v>
       </c>
       <c r="AW24" s="25"/>
       <c r="AX24" s="25"/>
       <c r="AY24" s="25">
         <f t="shared" si="13"/>
-        <v>0.85</v>
+        <v>-1.5</v>
       </c>
       <c r="AZ24" s="25">
         <f t="shared" si="14"/>
-        <v>0.15</v>
+        <v>2.5</v>
       </c>
       <c r="BA24" s="25">
         <f t="shared" si="15"/>
-        <v>0.85</v>
+        <v>-1.5</v>
       </c>
     </row>
     <row r="25" spans="2:53" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -4106,7 +4109,7 @@
         <v>54</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G30" s="24">
         <v>1</v>
@@ -4159,58 +4162,56 @@
         <v>1</v>
       </c>
       <c r="AE30" s="25"/>
-      <c r="AF30" s="25">
-        <v>0.25</v>
-      </c>
+      <c r="AF30" s="25"/>
       <c r="AG30" s="25">
         <f t="shared" ref="AG30:AG31" si="200">AD30-AF30</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AH30" s="25"/>
-      <c r="AI30" s="25"/>
+      <c r="AI30" s="25">
+        <v>1</v>
+      </c>
       <c r="AJ30" s="25">
         <f t="shared" ref="AJ30:AJ31" si="201">AG30-AI30</f>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="AK30" s="25"/>
       <c r="AL30" s="25"/>
       <c r="AM30" s="25">
         <f t="shared" ref="AM30:AM31" si="202">AJ30-AL30</f>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="AN30" s="25"/>
       <c r="AO30" s="25"/>
       <c r="AP30" s="25">
         <f t="shared" ref="AP30:AP31" si="203">AM30-AO30</f>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="AQ30" s="25"/>
       <c r="AR30" s="25"/>
       <c r="AS30" s="25">
         <f t="shared" ref="AS30:AS31" si="204">AP30-AR30</f>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="AT30" s="25"/>
-      <c r="AU30" s="25">
-        <v>0.15</v>
-      </c>
+      <c r="AU30" s="25"/>
       <c r="AV30" s="25">
         <f t="shared" ref="AV30:AV31" si="205">AS30-AU30</f>
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="AW30" s="25"/>
       <c r="AX30" s="25"/>
       <c r="AY30" s="25">
         <f t="shared" ref="AY30:AY31" si="206">AV30-AX30</f>
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="AZ30" s="25">
         <f t="shared" ref="AZ30:AZ31" si="207">H30+K30+N30+Q30+T30+W30+Z30+AC30+AF30+AI30+AL30+AO30+AR30+AU30+AX30</f>
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="BA30" s="25">
         <f t="shared" ref="BA30:BA31" si="208">G30-AZ30</f>
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:53" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -4514,64 +4515,62 @@
         <v>1</v>
       </c>
       <c r="AB33" s="25"/>
-      <c r="AC33" s="25"/>
+      <c r="AC33" s="25">
+        <v>2</v>
+      </c>
       <c r="AD33" s="25">
         <f t="shared" si="216"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AE33" s="25"/>
       <c r="AF33" s="25"/>
       <c r="AG33" s="25">
         <f t="shared" si="217"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AH33" s="25"/>
       <c r="AI33" s="25"/>
       <c r="AJ33" s="25">
         <f t="shared" si="218"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AK33" s="25"/>
       <c r="AL33" s="25"/>
       <c r="AM33" s="25">
         <f t="shared" si="219"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AN33" s="25"/>
       <c r="AO33" s="25"/>
       <c r="AP33" s="25">
         <f t="shared" si="220"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AQ33" s="25"/>
       <c r="AR33" s="25"/>
       <c r="AS33" s="25">
         <f t="shared" si="221"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AT33" s="25"/>
-      <c r="AU33" s="25">
-        <v>0.5</v>
-      </c>
+      <c r="AU33" s="25"/>
       <c r="AV33" s="25">
         <f t="shared" si="222"/>
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AW33" s="25"/>
-      <c r="AX33" s="25">
-        <v>0.5</v>
-      </c>
+      <c r="AX33" s="25"/>
       <c r="AY33" s="25">
         <f t="shared" si="223"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ33" s="25">
         <f t="shared" ref="AZ33" si="225">H33+K33+N33+Q33+T33+W33+Z33+AC33+AF33+AI33+AL33+AO33+AR33+AU33+AX33</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BA33" s="25">
         <f t="shared" si="224"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="34" spans="2:53" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -4830,7 +4829,7 @@
         <v>86</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="G36" s="19">
         <v>6</v>
@@ -5062,7 +5061,7 @@
         <v>54</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G38" s="24">
         <v>1</v>
@@ -5097,74 +5096,74 @@
         <v>1</v>
       </c>
       <c r="V38" s="25"/>
-      <c r="W38" s="25"/>
+      <c r="W38" s="25">
+        <v>0.5</v>
+      </c>
       <c r="X38" s="25">
         <f t="shared" si="214"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y38" s="25"/>
       <c r="Z38" s="25"/>
       <c r="AA38" s="25">
         <f t="shared" si="215"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AB38" s="25"/>
       <c r="AC38" s="25"/>
       <c r="AD38" s="25">
         <f t="shared" si="216"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AE38" s="25"/>
       <c r="AF38" s="25"/>
       <c r="AG38" s="25">
         <f t="shared" si="217"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AH38" s="25"/>
       <c r="AI38" s="25"/>
       <c r="AJ38" s="25">
         <f t="shared" si="218"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AK38" s="25"/>
-      <c r="AL38" s="25">
-        <v>0.25</v>
-      </c>
+      <c r="AL38" s="25"/>
       <c r="AM38" s="25">
         <f t="shared" si="219"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="AN38" s="25"/>
       <c r="AO38" s="25"/>
       <c r="AP38" s="25">
         <f t="shared" si="220"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="AQ38" s="25"/>
       <c r="AR38" s="25"/>
       <c r="AS38" s="25">
         <f t="shared" si="221"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="AT38" s="25"/>
       <c r="AU38" s="25"/>
       <c r="AV38" s="25">
         <f t="shared" si="222"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="AW38" s="25"/>
       <c r="AX38" s="25"/>
       <c r="AY38" s="25">
         <f t="shared" si="223"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="AZ38" s="25">
         <f>H38+K38+N38+Q38+T38+W38+Z38+AC38+AF38+AI38+AL38+AO38+AR38+AU38+AX38</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="BA38" s="25">
         <f t="shared" si="224"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="39" spans="2:53" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -5181,7 +5180,7 @@
         <v>54</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G39" s="24">
         <v>1</v>
@@ -5240,50 +5239,50 @@
         <v>1</v>
       </c>
       <c r="AH39" s="25"/>
-      <c r="AI39" s="25"/>
+      <c r="AI39" s="25">
+        <v>0.5</v>
+      </c>
       <c r="AJ39" s="25">
         <f t="shared" si="218"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AK39" s="25"/>
       <c r="AL39" s="25"/>
       <c r="AM39" s="25">
         <f t="shared" si="219"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN39" s="25"/>
       <c r="AO39" s="25"/>
       <c r="AP39" s="25">
         <f t="shared" si="220"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ39" s="25"/>
-      <c r="AR39" s="25">
-        <v>0.25</v>
-      </c>
+      <c r="AR39" s="25"/>
       <c r="AS39" s="25">
         <f t="shared" si="221"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="AT39" s="25"/>
       <c r="AU39" s="25"/>
       <c r="AV39" s="25">
         <f t="shared" si="222"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="AW39" s="25"/>
       <c r="AX39" s="25"/>
       <c r="AY39" s="25">
         <f t="shared" si="223"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="AZ39" s="25">
         <f t="shared" ref="AZ39" si="228">H39+K39+N39+Q39+T39+W39+Z39+AC39+AF39+AI39+AL39+AO39+AR39+AU39+AX39</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="BA39" s="25">
         <f t="shared" si="224"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="40" spans="2:53" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -5300,7 +5299,7 @@
         <v>54</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G40" s="24">
         <v>1</v>
@@ -5335,76 +5334,74 @@
         <v>1</v>
       </c>
       <c r="V40" s="25"/>
-      <c r="W40" s="25"/>
+      <c r="W40" s="25">
+        <v>0.75</v>
+      </c>
       <c r="X40" s="25">
         <f t="shared" si="214"/>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="Y40" s="25"/>
       <c r="Z40" s="25"/>
       <c r="AA40" s="25">
         <f t="shared" si="215"/>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="AB40" s="25"/>
-      <c r="AC40" s="25">
-        <v>0.5</v>
-      </c>
+      <c r="AC40" s="25"/>
       <c r="AD40" s="25">
         <f t="shared" si="216"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AE40" s="25"/>
       <c r="AF40" s="25"/>
       <c r="AG40" s="25">
         <f t="shared" si="217"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AH40" s="25"/>
       <c r="AI40" s="25"/>
       <c r="AJ40" s="25">
         <f t="shared" si="218"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AK40" s="25"/>
       <c r="AL40" s="25"/>
       <c r="AM40" s="25">
         <f t="shared" si="219"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AN40" s="25"/>
       <c r="AO40" s="25"/>
       <c r="AP40" s="25">
         <f t="shared" si="220"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AQ40" s="25"/>
       <c r="AR40" s="25"/>
       <c r="AS40" s="25">
         <f t="shared" si="221"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AT40" s="25"/>
-      <c r="AU40" s="25">
-        <v>0.15</v>
-      </c>
+      <c r="AU40" s="25"/>
       <c r="AV40" s="25">
         <f t="shared" si="222"/>
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="AW40" s="25"/>
       <c r="AX40" s="25"/>
       <c r="AY40" s="25">
         <f t="shared" si="223"/>
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="AZ40" s="25">
         <f>H40+K40+N40+Q40+T40+W40+Z40+AC40+AF40+AI40+AL40+AO40+AR40+AU40+AX40</f>
-        <v>0.65</v>
+        <v>0.75</v>
       </c>
       <c r="BA40" s="25">
         <f t="shared" si="224"/>
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="41" spans="2:53" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -5421,7 +5418,7 @@
         <v>54</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G41" s="24">
         <v>1</v>
@@ -5469,61 +5466,61 @@
       </c>
       <c r="AB41" s="25"/>
       <c r="AC41" s="25">
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="AD41" s="25">
         <f t="shared" si="216"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AE41" s="25"/>
       <c r="AF41" s="25"/>
       <c r="AG41" s="25">
         <f t="shared" si="217"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AH41" s="25"/>
       <c r="AI41" s="25"/>
       <c r="AJ41" s="25">
         <f t="shared" si="218"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AK41" s="25"/>
       <c r="AL41" s="25"/>
       <c r="AM41" s="25">
         <f t="shared" si="219"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AN41" s="25"/>
       <c r="AO41" s="25"/>
       <c r="AP41" s="25">
         <f t="shared" si="220"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AQ41" s="25"/>
       <c r="AR41" s="25"/>
       <c r="AS41" s="25">
         <f t="shared" si="221"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AT41" s="25"/>
       <c r="AU41" s="25"/>
       <c r="AV41" s="25">
         <f t="shared" si="222"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AW41" s="25"/>
       <c r="AX41" s="25"/>
       <c r="AY41" s="25">
         <f t="shared" si="223"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AZ41" s="25">
         <f t="shared" ref="AZ41" si="229">H41+K41+N41+Q41+T41+W41+Z41+AC41+AF41+AI41+AL41+AO41+AR41+AU41+AX41</f>
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="BA41" s="25">
         <f t="shared" si="224"/>
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="42" spans="2:53" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -6902,6 +6899,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -6913,11 +6915,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización de modelo de dominio, Modelo relacional, Script de BD
</commit_message>
<xml_diff>
--- a/Documentos/Tareas/Iteración_2 Registro.xlsx
+++ b/Documentos/Tareas/Iteración_2 Registro.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymu\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Documents\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BDF962-6908-4247-BCEC-9A0018B53793}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="96">
   <si>
     <t>Columna</t>
   </si>
@@ -315,16 +314,13 @@
   </si>
   <si>
     <t>CU - 24</t>
-  </si>
-  <si>
-    <t>Por iniciar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +352,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -495,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -617,6 +628,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,10 +979,10 @@
   <dimension ref="B1:BA54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AI6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AJ31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E43" sqref="E43"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,7 +2236,7 @@
         <v>53</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="G14" s="33">
         <v>1</v>
@@ -2292,24 +2319,28 @@
         <v>1</v>
       </c>
       <c r="AT14" s="34"/>
-      <c r="AU14" s="34"/>
+      <c r="AU14" s="34">
+        <v>0.5</v>
+      </c>
       <c r="AV14" s="34">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW14" s="34"/>
-      <c r="AX14" s="34"/>
+      <c r="AX14" s="34">
+        <v>0.7</v>
+      </c>
       <c r="AY14" s="34">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>-0.19999999999999996</v>
       </c>
       <c r="AZ14" s="34">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="BA14" s="34">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>-0.19999999999999996</v>
       </c>
     </row>
     <row r="15" spans="2:53" x14ac:dyDescent="0.25">
@@ -2546,121 +2577,121 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="17" spans="2:53" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="27"/>
-      <c r="C17" s="28" t="s">
+    <row r="17" spans="2:53" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="47"/>
+      <c r="C17" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="30">
-        <v>1</v>
-      </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31">
+      <c r="F17" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="50">
+        <v>1</v>
+      </c>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51">
         <f>G17-H17</f>
         <v>1</v>
       </c>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31">
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51">
         <f t="shared" ref="L17" si="97">I17-K17</f>
         <v>1</v>
       </c>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31">
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="51">
         <f t="shared" ref="O17" si="98">L17-N17</f>
         <v>1</v>
       </c>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31">
+      <c r="P17" s="51"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="51">
         <f t="shared" ref="R17" si="99">O17-Q17</f>
         <v>1</v>
       </c>
-      <c r="S17" s="31"/>
-      <c r="T17" s="31"/>
-      <c r="U17" s="31">
+      <c r="S17" s="51"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="51">
         <f t="shared" ref="U17" si="100">R17-T17</f>
         <v>1</v>
       </c>
-      <c r="V17" s="31"/>
-      <c r="W17" s="31"/>
-      <c r="X17" s="31">
+      <c r="V17" s="51"/>
+      <c r="W17" s="51"/>
+      <c r="X17" s="51">
         <f t="shared" ref="X17" si="101">U17-W17</f>
         <v>1</v>
       </c>
-      <c r="Y17" s="31"/>
-      <c r="Z17" s="31"/>
-      <c r="AA17" s="31">
+      <c r="Y17" s="51"/>
+      <c r="Z17" s="51"/>
+      <c r="AA17" s="51">
         <f t="shared" ref="AA17" si="102">X17-Z17</f>
         <v>1</v>
       </c>
-      <c r="AB17" s="31"/>
-      <c r="AC17" s="31"/>
-      <c r="AD17" s="31">
+      <c r="AB17" s="51"/>
+      <c r="AC17" s="51"/>
+      <c r="AD17" s="51">
         <f t="shared" ref="AD17" si="103">AA17-AC17</f>
         <v>1</v>
       </c>
-      <c r="AE17" s="31"/>
-      <c r="AF17" s="31"/>
-      <c r="AG17" s="31">
+      <c r="AE17" s="51"/>
+      <c r="AF17" s="51"/>
+      <c r="AG17" s="51">
         <f t="shared" ref="AG17" si="104">AD17-AF17</f>
         <v>1</v>
       </c>
-      <c r="AH17" s="31"/>
-      <c r="AI17" s="31"/>
-      <c r="AJ17" s="31">
+      <c r="AH17" s="51"/>
+      <c r="AI17" s="51"/>
+      <c r="AJ17" s="51">
         <f t="shared" ref="AJ17" si="105">AG17-AI17</f>
         <v>1</v>
       </c>
-      <c r="AK17" s="31"/>
-      <c r="AL17" s="31"/>
-      <c r="AM17" s="31">
+      <c r="AK17" s="51"/>
+      <c r="AL17" s="51"/>
+      <c r="AM17" s="51">
         <f t="shared" ref="AM17" si="106">AJ17-AL17</f>
         <v>1</v>
       </c>
-      <c r="AN17" s="31"/>
-      <c r="AO17" s="31"/>
-      <c r="AP17" s="31">
+      <c r="AN17" s="51"/>
+      <c r="AO17" s="51"/>
+      <c r="AP17" s="51">
         <f t="shared" ref="AP17" si="107">AM17-AO17</f>
         <v>1</v>
       </c>
-      <c r="AQ17" s="31"/>
-      <c r="AR17" s="31"/>
-      <c r="AS17" s="31">
+      <c r="AQ17" s="51"/>
+      <c r="AR17" s="51"/>
+      <c r="AS17" s="51">
         <f t="shared" ref="AS17" si="108">AP17-AR17</f>
         <v>1</v>
       </c>
-      <c r="AT17" s="31"/>
-      <c r="AU17" s="31">
+      <c r="AT17" s="51"/>
+      <c r="AU17" s="51">
         <v>0.25</v>
       </c>
-      <c r="AV17" s="31">
+      <c r="AV17" s="51">
         <f t="shared" ref="AV17" si="109">AS17-AU17</f>
         <v>0.75</v>
       </c>
-      <c r="AW17" s="31"/>
-      <c r="AX17" s="31">
+      <c r="AW17" s="51"/>
+      <c r="AX17" s="51">
         <v>0.25</v>
       </c>
-      <c r="AY17" s="31">
+      <c r="AY17" s="51">
         <f t="shared" ref="AY17" si="110">AV17-AX17</f>
         <v>0.5</v>
       </c>
-      <c r="AZ17" s="31">
+      <c r="AZ17" s="51">
         <f t="shared" ref="AZ17" si="111">H17+K17+N17+Q17+T17+W17+Z17+AC17+AF17+AI17+AL17+AO17+AR17+AU17+AX17</f>
         <v>0.5</v>
       </c>
-      <c r="BA17" s="31">
+      <c r="BA17" s="51">
         <f t="shared" ref="BA17" si="112">G17-AZ17</f>
         <v>0.5</v>
       </c>
@@ -4944,7 +4975,7 @@
         <v>53</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G37" s="33">
         <v>1</v>
@@ -5033,18 +5064,20 @@
         <v>1</v>
       </c>
       <c r="AW37" s="34"/>
-      <c r="AX37" s="34"/>
+      <c r="AX37" s="34">
+        <v>1.5</v>
+      </c>
       <c r="AY37" s="34">
         <f t="shared" si="223"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AZ37" s="34">
         <f t="shared" ref="AZ37" si="227">H37+K37+N37+Q37+T37+W37+Z37+AC37+AF37+AI37+AL37+AO37+AR37+AU37+AX37</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="BA37" s="34">
         <f t="shared" si="224"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="38" spans="2:53" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -6899,11 +6932,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -6915,6 +6943,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>